<commit_message>
Move pre/final manifests into a single Excel file
Use a single Excel file with tabs for pre and final manifests.  Add
config to represent which Hubs do not have ULNs.  Add user dialogs to
get ULN info.  Write Hub-based passenger listings in the final manifest.
Still need to prioritize the Hub-based passenger lists and assign
passengers to the ULN based on number of available seats.  Also need to
add styling and ULN usage text boxes, and copying of Instructions tab.
</commit_message>
<xml_diff>
--- a/CRC_Manifest_Processor_Config.xlsx
+++ b/CRC_Manifest_Processor_Config.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="19020" windowHeight="11895" activeTab="3"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="19020" windowHeight="11895" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="DestinationHubCountry" sheetId="1" r:id="rId1"/>
     <sheet name="LocationAlias" sheetId="2" r:id="rId2"/>
     <sheet name="PriorityMOS" sheetId="3" r:id="rId3"/>
     <sheet name="RankComparison" sheetId="4" r:id="rId4"/>
+    <sheet name="HubsWithoutUlns" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="994" uniqueCount="503">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1004" uniqueCount="509">
   <si>
     <t>FINAL_DESTINATION</t>
   </si>
@@ -1526,6 +1527,24 @@
   </si>
   <si>
     <t>GS-6</t>
+  </si>
+  <si>
+    <t>HUBS_WITHOUT_ULNS</t>
+  </si>
+  <si>
+    <t>SHIRANA</t>
+  </si>
+  <si>
+    <t>BASYAH</t>
+  </si>
+  <si>
+    <t>BASRA</t>
+  </si>
+  <si>
+    <t>UNKNOWN</t>
+  </si>
+  <si>
+    <t>NOT_FOUND</t>
   </si>
 </sst>
 </file>
@@ -2398,8 +2417,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C199"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView topLeftCell="A148" workbookViewId="0">
+      <selection activeCell="B181" sqref="B181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -4164,7 +4183,7 @@
         <v>173</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C160" s="1" t="s">
         <v>172</v>
@@ -4296,7 +4315,7 @@
         <v>186</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C172" s="1" t="s">
         <v>172</v>
@@ -4318,7 +4337,7 @@
         <v>188</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C174" s="1" t="s">
         <v>172</v>
@@ -4439,7 +4458,7 @@
         <v>197</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C185" s="1" t="s">
         <v>172</v>
@@ -4610,11 +4629,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B76"/>
+  <dimension ref="A1:B79"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
@@ -4657,55 +4674,55 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>205</v>
+        <v>506</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>34</v>
+        <v>179</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="1" t="s">
-        <v>207</v>
+      <c r="A7" s="2" t="s">
+        <v>505</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>45</v>
+        <v>179</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>50</v>
@@ -4713,7 +4730,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>50</v>
@@ -4721,7 +4738,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>50</v>
@@ -4729,7 +4746,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>50</v>
@@ -4737,7 +4754,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>50</v>
@@ -4745,39 +4762,39 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>50</v>
@@ -4785,39 +4802,39 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>72</v>
@@ -4825,79 +4842,79 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>74</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" s="4" t="s">
-        <v>391</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="1" t="s">
-        <v>229</v>
+      <c r="A30" s="4" t="s">
+        <v>391</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>151</v>
+        <v>64</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>151</v>
+        <v>64</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>88</v>
+        <v>151</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>88</v>
+        <v>151</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>88</v>
@@ -4905,7 +4922,7 @@
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>88</v>
@@ -4913,23 +4930,23 @@
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="1" t="s">
-        <v>91</v>
+        <v>235</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>91</v>
@@ -4937,7 +4954,7 @@
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="1" t="s">
-        <v>238</v>
+        <v>91</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>91</v>
@@ -4945,63 +4962,63 @@
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>103</v>
@@ -5009,23 +5026,23 @@
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>104</v>
@@ -5033,7 +5050,7 @@
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>104</v>
@@ -5041,103 +5058,103 @@
     </row>
     <row r="53" spans="1:2">
       <c r="A53" s="1" t="s">
-        <v>108</v>
+        <v>249</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>251</v>
+        <v>104</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>251</v>
+        <v>104</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" s="1" t="s">
-        <v>253</v>
+        <v>108</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>110</v>
+        <v>251</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>110</v>
+        <v>251</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>91</v>
+        <v>110</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>91</v>
+        <v>118</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" s="1" t="s">
-        <v>127</v>
+        <v>256</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>251</v>
+        <v>91</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>138</v>
+        <v>91</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" s="1" t="s">
-        <v>259</v>
+        <v>127</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>138</v>
+        <v>251</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>137</v>
@@ -5145,7 +5162,7 @@
     </row>
     <row r="66" spans="1:2">
       <c r="A66" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>137</v>
@@ -5153,89 +5170,114 @@
     </row>
     <row r="67" spans="1:2">
       <c r="A67" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" s="1" t="s">
-        <v>395</v>
+        <v>264</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" s="1" t="s">
-        <v>267</v>
+        <v>395</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>175</v>
+        <v>144</v>
       </c>
     </row>
     <row r="74" spans="1:2">
-      <c r="A74" s="1" t="s">
-        <v>270</v>
+      <c r="A74" s="2" t="s">
+        <v>504</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>167</v>
+        <v>151</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" s="1" t="s">
         <v>394</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="B79" s="1" t="s">
         <v>169</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:B76">
-    <sortCondition ref="A2"/>
+  <sortState ref="A2:B79">
+    <sortCondition ref="A2:A79"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5857,8 +5899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B141"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -6995,4 +7037,43 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="26" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="7" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="1" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="1" t="s">
+        <v>508</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fix Record.compareTo bug; upgrade to POI 3.8 b4
Fixed a bug in Record.compareTo method that was causing
PrioritizedRecords to lose Records.  Only Record.equal should nearly
match compareTo() == 0 now.  Upgraded to POI 3.8 beta 4 since it claims
to fix a bug in cloning CellStyles across workbooks.  Previously it
would copy some of the style (Fonts, but not borders and colors), but
leave the workbook styles in an inconsistent state.  Now it does not
corrupt the workbook styles, but does not copy any of the style. :(

Perhaps I will see if fixing the Apache POI bug is not too hard to do.
</commit_message>
<xml_diff>
--- a/CRC_Manifest_Processor_Config.xlsx
+++ b/CRC_Manifest_Processor_Config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="19020" windowHeight="11895" activeTab="4"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="19020" windowHeight="11895" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="DestinationHubCountry" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1004" uniqueCount="509">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1006" uniqueCount="510">
   <si>
     <t>FINAL_DESTINATION</t>
   </si>
@@ -1545,6 +1545,9 @@
   </si>
   <si>
     <t>NOT_FOUND</t>
+  </si>
+  <si>
+    <t>BAGDAD</t>
   </si>
 </sst>
 </file>
@@ -2417,8 +2420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C199"/>
   <sheetViews>
-    <sheetView topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="B181" sqref="B181"/>
+    <sheetView topLeftCell="A151" workbookViewId="0">
+      <selection activeCell="B165" sqref="B165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -4183,7 +4186,7 @@
         <v>173</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C160" s="1" t="s">
         <v>172</v>
@@ -4194,7 +4197,7 @@
         <v>175</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C161" s="1" t="s">
         <v>172</v>
@@ -4205,7 +4208,7 @@
         <v>177</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C162" s="1" t="s">
         <v>172</v>
@@ -4216,7 +4219,7 @@
         <v>178</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C163" s="1" t="s">
         <v>172</v>
@@ -4238,7 +4241,7 @@
         <v>176</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C165" s="1" t="s">
         <v>172</v>
@@ -4249,7 +4252,7 @@
         <v>180</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C166" s="1" t="s">
         <v>172</v>
@@ -4260,7 +4263,7 @@
         <v>181</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C167" s="1" t="s">
         <v>172</v>
@@ -4271,7 +4274,7 @@
         <v>182</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C168" s="1" t="s">
         <v>172</v>
@@ -4282,7 +4285,7 @@
         <v>183</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C169" s="1" t="s">
         <v>172</v>
@@ -4304,7 +4307,7 @@
         <v>185</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C171" s="1" t="s">
         <v>172</v>
@@ -4315,7 +4318,7 @@
         <v>186</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C172" s="1" t="s">
         <v>172</v>
@@ -4326,7 +4329,7 @@
         <v>187</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C173" s="1" t="s">
         <v>172</v>
@@ -4337,7 +4340,7 @@
         <v>188</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C174" s="1" t="s">
         <v>172</v>
@@ -4348,7 +4351,7 @@
         <v>189</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C175" s="1" t="s">
         <v>172</v>
@@ -4359,7 +4362,7 @@
         <v>190</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C176" s="1" t="s">
         <v>172</v>
@@ -4381,7 +4384,7 @@
         <v>192</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C178" s="1" t="s">
         <v>172</v>
@@ -4425,7 +4428,7 @@
         <v>195</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C182" s="1" t="s">
         <v>172</v>
@@ -4436,7 +4439,7 @@
         <v>196</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C183" s="1" t="s">
         <v>172</v>
@@ -4447,7 +4450,7 @@
         <v>13</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C184" s="1" t="s">
         <v>172</v>
@@ -4458,7 +4461,7 @@
         <v>197</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C185" s="1" t="s">
         <v>172</v>
@@ -4469,7 +4472,7 @@
         <v>198</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C186" s="1" t="s">
         <v>172</v>
@@ -4629,9 +4632,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B79"/>
+  <dimension ref="A1:B80"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
@@ -4674,47 +4679,47 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>506</v>
+        <v>509</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="2" t="s">
+    <row r="8" spans="1:2">
+      <c r="A8" s="2" t="s">
         <v>505</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>179</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>45</v>
@@ -4722,15 +4727,15 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>50</v>
@@ -4738,7 +4743,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>50</v>
@@ -4746,7 +4751,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>50</v>
@@ -4754,7 +4759,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>50</v>
@@ -4762,7 +4767,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>50</v>
@@ -4770,7 +4775,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>50</v>
@@ -4778,15 +4783,15 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>46</v>
@@ -4794,15 +4799,15 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>50</v>
@@ -4810,7 +4815,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>50</v>
@@ -4818,31 +4823,31 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>72</v>
@@ -4850,7 +4855,7 @@
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>72</v>
@@ -4858,39 +4863,39 @@
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="4" t="s">
         <v>391</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B31" s="1" t="s">
         <v>81</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>64</v>
@@ -4898,15 +4903,15 @@
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>151</v>
+        <v>64</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>151</v>
@@ -4914,15 +4919,15 @@
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>88</v>
+        <v>151</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>88</v>
@@ -4930,7 +4935,7 @@
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>88</v>
@@ -4938,7 +4943,7 @@
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>88</v>
@@ -4946,15 +4951,15 @@
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="1" t="s">
-        <v>91</v>
+        <v>236</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>91</v>
@@ -4962,7 +4967,7 @@
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="1" t="s">
-        <v>237</v>
+        <v>91</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>91</v>
@@ -4970,7 +4975,7 @@
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>91</v>
@@ -4978,31 +4983,31 @@
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>99</v>
@@ -5010,23 +5015,23 @@
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>103</v>
@@ -5034,7 +5039,7 @@
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>103</v>
@@ -5042,15 +5047,15 @@
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>104</v>
@@ -5058,7 +5063,7 @@
     </row>
     <row r="53" spans="1:2">
       <c r="A53" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>104</v>
@@ -5066,7 +5071,7 @@
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>104</v>
@@ -5074,15 +5079,15 @@
     </row>
     <row r="55" spans="1:2">
       <c r="A55" s="1" t="s">
-        <v>108</v>
+        <v>250</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>251</v>
+        <v>104</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" s="1" t="s">
-        <v>252</v>
+        <v>108</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>251</v>
@@ -5090,15 +5095,15 @@
     </row>
     <row r="57" spans="1:2">
       <c r="A57" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>110</v>
+        <v>251</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>110</v>
@@ -5106,23 +5111,23 @@
     </row>
     <row r="59" spans="1:2">
       <c r="A59" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>91</v>
+        <v>118</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>91</v>
@@ -5130,23 +5135,23 @@
     </row>
     <row r="62" spans="1:2">
       <c r="A62" s="1" t="s">
-        <v>127</v>
+        <v>257</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>251</v>
+        <v>91</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" s="1" t="s">
-        <v>258</v>
+        <v>127</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>138</v>
+        <v>251</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>138</v>
@@ -5154,15 +5159,15 @@
     </row>
     <row r="65" spans="1:2">
       <c r="A65" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>137</v>
@@ -5170,7 +5175,7 @@
     </row>
     <row r="67" spans="1:2">
       <c r="A67" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>137</v>
@@ -5178,7 +5183,7 @@
     </row>
     <row r="68" spans="1:2">
       <c r="A68" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>137</v>
@@ -5186,15 +5191,15 @@
     </row>
     <row r="69" spans="1:2">
       <c r="A69" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>138</v>
@@ -5202,73 +5207,81 @@
     </row>
     <row r="71" spans="1:2">
       <c r="A71" s="1" t="s">
-        <v>395</v>
+        <v>265</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" s="1" t="s">
-        <v>266</v>
+        <v>395</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="B73" s="1" t="s">
+      <c r="B74" s="1" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="74" spans="1:2">
-      <c r="A74" s="2" t="s">
+    <row r="75" spans="1:2">
+      <c r="A75" s="2" t="s">
         <v>504</v>
       </c>
-      <c r="B74" s="1" t="s">
+      <c r="B75" s="1" t="s">
         <v>141</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2">
-      <c r="A75" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>175</v>
+        <v>151</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>154</v>
+        <v>175</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" s="1" t="s">
         <v>394</v>
       </c>
-      <c r="B79" s="1" t="s">
+      <c r="B80" s="1" t="s">
         <v>169</v>
       </c>
     </row>
@@ -7043,7 +7056,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Final changes for version 1.0
Added documentation to config Excel file.  Turned off attempts to copy
the Instructions tab to the generated manifests.  Apache POI Cell Style
clone bug is not resolved and there is not an easy way to copy text
boxes, so we will not do this for now.
</commit_message>
<xml_diff>
--- a/CRC_Manifest_Processor_Config.xlsx
+++ b/CRC_Manifest_Processor_Config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="19020" windowHeight="11895" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="19020" windowHeight="11895"/>
   </bookViews>
   <sheets>
     <sheet name="DestinationHubCountry" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1006" uniqueCount="510">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1010" uniqueCount="512">
   <si>
     <t>FINAL_DESTINATION</t>
   </si>
@@ -1548,6 +1548,12 @@
   </si>
   <si>
     <t>BAGDAD</t>
+  </si>
+  <si>
+    <t>KNB</t>
+  </si>
+  <si>
+    <t>CAMP PATRIOT</t>
   </si>
 </sst>
 </file>
@@ -2133,6 +2139,963 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5467350" y="190500"/>
+          <a:ext cx="6162675" cy="9610725"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" u="sng">
+              <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>Destination Hub Country</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" u="sng" baseline="0">
+              <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t> Configuration</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1400" b="1" baseline="0">
+            <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+            <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" baseline="0">
+              <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>This sheet has the data that represents final destinations in theater and how passengers get to their destination.  Description of the columns:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1200" b="0" baseline="0">
+            <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+            <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="1" baseline="0">
+              <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>FINAL_DESTINATION</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" baseline="0">
+              <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>:  The camp, FOB, COP, base, or office where the passenger is going.  This is used to determine the major air hub that the passenger will travel through and the country where the destination is found.  The final destination should be unique so that there is no confusion.  Sometimes there are alternate spellings for a final destination.  These are found in the LocationAlias sheet.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1200" b="0" baseline="0">
+            <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+            <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="1" baseline="0">
+              <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>HUB</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" baseline="0">
+              <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>:  The major air hub that is used to reach the final destination.  The total number of passengers going to this hub will be used to reserve seats for intra-theater flights from the Theater Gateway to the major air hub.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1200" b="0" baseline="0">
+            <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+            <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="1" baseline="0">
+              <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>COUNTRY</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" baseline="0">
+              <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>:  The country where the final destination is located.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1200" b="0" baseline="0">
+            <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+            <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" baseline="0">
+              <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>This sheet should be checked each month against E-Channel updates.  If the major air hub to a destination changes, the HUB column should be updated.  If there are new final destinations, they should be added to the bottom of the list.  The major air hub for new final destinations can be found using Google.  Use Google to find the approximate location of the final destination and then find the nearest major air hub.  </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1200" b="0" baseline="0">
+            <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+            <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>If you get a NOT_FOUND hub result in the generated manifest, it means that the final destination is not in this list (the Destination Hub Country Configuration) and will need to be added as a new final destination.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1200" b="0" baseline="0">
+            <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+            <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1200" b="0" baseline="0">
+            <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+            <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" baseline="0">
+              <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>For example, suppose we get a new final destination in Jazah, Afghanistan.  Search Google for "Jazah, Afghanistan".  Many of the results show that Jazah is near Kandahar.  Since no other air hubs are closer, put KANDAHAR in the HUB column.  This means that the new entry would be:  </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" baseline="0">
+              <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>FINAL_DESTINATION:  JAZAH</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" baseline="0">
+              <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>HUB:  KANDAHAR</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" baseline="0">
+              <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>COUNTRY:  AFGHANISTAN</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1200" b="0" baseline="0">
+            <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+            <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" baseline="0">
+              <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>If you get a UNKNOWN hub result in the generated manifest, it means that the passenger put UNKNOWN in their final destination or left their final destination blank.  If the final destination is not known, we cannot determine what major air hub, so the HUB column will be UNKNOWN.  Passengers with UNKNOWN hubs will not have seats reserved on intra-theater flights and must travel by standby.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1200" b="0" baseline="0">
+            <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+            <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" baseline="0">
+              <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>The exception to this rule is medical personnel travelling to Afghanistan.  Medical personnel with UNKNOWN final destinations in Afghanistan will travel to BAGRAM to get final duty locations assigned.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1400" b="1" baseline="0">
+            <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1400" b="0">
+            <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1400" b="0">
+            <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1400" b="0">
+            <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+            <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5172075" y="161925"/>
+          <a:ext cx="6334125" cy="6886575"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" u="sng">
+              <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>Location Alias Configuration</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1200" b="1" u="sng">
+            <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+            <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1200">
+            <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+            <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>This</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" baseline="0">
+              <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t> sheet has alternate names and alternate spellings for final destinations in theater.  There are several reasons for this given below.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1200" baseline="0">
+            <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+            <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="1" baseline="0">
+              <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>Reason #1:  Names from other languages</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" baseline="0">
+              <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>:  Many of the names of final destinations in theater come from other languages (Arabic, Farsi, Pashtu, Urdu, etc.).  Since these languages have non-English alphabets, we use the way the name sounds to create an English spelling for the name.  In many cases there are multiple correct spellings for a location.  For example, see the "other names" from this Wikipedia article:  http://en.wikipedia.org/wiki/Khanashin</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1200">
+            <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+            <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1200">
+            <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+            <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="1">
+              <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>Reason #2:</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="1" baseline="0">
+              <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>  Multiple names for a destination</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" baseline="0">
+              <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>:  Many of the final destinations where we work have more than one name.  For example, Camp Patriot, Kuwait is also called Kuwait Naval Base.  </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1200" baseline="0">
+            <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+            <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="1" baseline="0">
+              <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>Reason #3:  Spelling Errors</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" baseline="0">
+              <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>:  Sometimes passengers deploying into theater do not know the correct spelling of their destination.  Some misspellings are so common that they are worth adding to this list to prevent NOT_FOUND results.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1200">
+            <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+            <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1200">
+            <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+            <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1200">
+            <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+            <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="1">
+              <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>!! IMPORTANT !!</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>All</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" baseline="0">
+              <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t> names in the FINAL_DESTINATION column on this sheet must have corresponding entries in the Destination Hub Country sheet.  The spellings in the FINAL_DESTINATION column on this sheet must match the spellings in the FINAL_DESTINATION column of the Destination Hub Country sheet. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1200" baseline="0">
+            <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+            <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="1" baseline="0">
+              <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>All of the location aliases in the manifest provided by the CRC will be replaced with the final destinations in this list.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1">
+            <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+            <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+            <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1400">
+            <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+            <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="904875" y="219075"/>
+          <a:ext cx="7219950" cy="5391150"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" u="sng">
+              <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>Priority MOS Configuration</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1400" b="1" u="sng">
+            <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+            <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" u="none">
+              <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>This sheet has a list of MOS's</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" u="none" baseline="0">
+              <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t> that are high priority.  This is usually medical MOS's, but may include other MOS's as well.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1200" b="0" u="none" baseline="0">
+            <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+            <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" u="none" baseline="0">
+              <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>As a rule, many medical service providers (doctors, nurses, etc.) usually have short deployment orders so it is important to get them into theater as quickly as possible.  For this reason, passengers with high priority MOS's will be given reserved seats before passengers who do not have a high priority MOS.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1200" b="0" u="none" baseline="0">
+            <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+            <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" u="none" baseline="0">
+              <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>On the final manifest, if there are fewer seats available than there are passengers going to a major air hub, passengers with a high priority MOS will get the seats first.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1200" b="0" u="none" baseline="0">
+            <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+            <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" u="none" baseline="0">
+              <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>This sheet will only need to be updated if other (non-medical) MOS's are marked as high priority or if the MOS code changes.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1200" b="0" u="none"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1438275" y="180975"/>
+          <a:ext cx="6734175" cy="5734050"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" u="sng">
+              <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>Rank Comparison Configuration</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1400" b="0" u="none">
+            <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+            <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1400" b="0" u="none">
+            <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+            <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" u="none">
+              <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>This</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" u="none" baseline="0">
+              <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t> sheet has a list of all of the rank abbrevations for each branch of the US Armed Forces and also DoD Civilian pay grades.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1200" b="0" u="none" baseline="0">
+            <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+            <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" u="none" baseline="0">
+              <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>Each of the ranks / rates / pay grades is mapped to a level that corresponds to a priority for travel.  Higher-ranking passengers will be given priority over lower-ranking passengers unless the lower-ranking passengers have a priority MOS.  (See the Priority MOS sheet.)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1200" b="0" u="none" baseline="0">
+            <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+            <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" u="none" baseline="0">
+              <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>This sheet should not need to be updated unless there are changes in the ranks / rates of an Armed Forces service branch.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1200" b="0" u="none">
+            <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+            <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1990725" y="238125"/>
+          <a:ext cx="5705475" cy="4238625"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" u="sng">
+              <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>Hubs Without ULNs Configuration</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1400">
+            <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+            <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>This sheet is a list of hubs</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" baseline="0">
+              <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t> that should not have their own tab in the generated final manifest.  There are two reasons for this:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1200" baseline="0">
+            <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+            <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="1" baseline="0">
+              <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>Reason #1:  Hub is the Theater Gateway</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" baseline="0">
+              <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>:  Hubs that are the Theater Gateway will not need onward movement intra-theater flights.  Passengers whose major air hub is the Theater Gateway will travel by ground transportation to their final destination.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1200" baseline="0">
+            <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+            <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="1" baseline="0">
+              <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>Reason #2:  Not really a major air hub</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" baseline="0">
+              <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>:  UNKNOWN and NOT_FOUND are not real major air hubs.  UNKNOWN is placed in the HUB column for passengers who do not know their final destination in theater, so no air hub lookup is possible.  NOT_FOUND is placed in the HUB column when the passenger has a final destination that is not in the Destination Hub Country Configuration.  If any passengers have NOT_FOUND in the HUB column, their final destination's hub will need to be found and the Destination Hub Country Configuration will need to be updated.  (See the Destination Hub Country Configuration for more details.)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1200">
+            <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+            <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2420,9 +3383,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C199"/>
   <sheetViews>
-    <sheetView topLeftCell="A151" workbookViewId="0">
-      <selection activeCell="B165" sqref="B165"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
@@ -4627,16 +5588,15 @@
     <sortCondition ref="A2:A199"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B80"/>
+  <dimension ref="A1:B82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
@@ -4671,18 +5631,18 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>174</v>
+        <v>509</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>509</v>
+        <v>174</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -4719,15 +5679,15 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
-        <v>207</v>
+        <v>511</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>45</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>45</v>
@@ -4735,15 +5695,15 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>50</v>
@@ -4751,7 +5711,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>50</v>
@@ -4759,7 +5719,7 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>50</v>
@@ -4767,7 +5727,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>50</v>
@@ -4775,7 +5735,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>50</v>
@@ -4783,7 +5743,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>50</v>
@@ -4791,15 +5751,15 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>46</v>
@@ -4807,15 +5767,15 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>50</v>
@@ -4823,7 +5783,7 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>50</v>
@@ -4831,31 +5791,31 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>72</v>
@@ -4863,7 +5823,7 @@
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>72</v>
@@ -4871,39 +5831,39 @@
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31" s="4" t="s">
+      <c r="A31" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="4" t="s">
         <v>391</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B32" s="1" t="s">
         <v>81</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>64</v>
@@ -4911,15 +5871,15 @@
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>151</v>
+        <v>64</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>151</v>
@@ -4927,15 +5887,15 @@
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>88</v>
+        <v>151</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>88</v>
@@ -4943,7 +5903,7 @@
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>88</v>
@@ -4951,7 +5911,7 @@
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>88</v>
@@ -4959,23 +5919,23 @@
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="1" t="s">
-        <v>91</v>
+        <v>510</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>91</v>
+        <v>10</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>91</v>
@@ -4983,7 +5943,7 @@
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="1" t="s">
-        <v>238</v>
+        <v>91</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>91</v>
@@ -4991,63 +5951,63 @@
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>103</v>
@@ -5055,23 +6015,23 @@
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>104</v>
@@ -5079,7 +6039,7 @@
     </row>
     <row r="55" spans="1:2">
       <c r="A55" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>104</v>
@@ -5087,103 +6047,103 @@
     </row>
     <row r="56" spans="1:2">
       <c r="A56" s="1" t="s">
-        <v>108</v>
+        <v>249</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>251</v>
+        <v>104</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>251</v>
+        <v>104</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" s="1" t="s">
-        <v>253</v>
+        <v>108</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>110</v>
+        <v>251</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>110</v>
+        <v>251</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>91</v>
+        <v>110</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>91</v>
+        <v>118</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" s="1" t="s">
-        <v>127</v>
+        <v>256</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>251</v>
+        <v>91</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>138</v>
+        <v>91</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" s="1" t="s">
-        <v>259</v>
+        <v>127</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>138</v>
+        <v>251</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>137</v>
@@ -5191,7 +6151,7 @@
     </row>
     <row r="69" spans="1:2">
       <c r="A69" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>137</v>
@@ -5199,98 +6159,115 @@
     </row>
     <row r="70" spans="1:2">
       <c r="A70" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" s="1" t="s">
-        <v>395</v>
+        <v>264</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" s="1" t="s">
-        <v>267</v>
+        <v>395</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
     </row>
     <row r="75" spans="1:2">
-      <c r="A75" s="2" t="s">
-        <v>504</v>
+      <c r="A75" s="1" t="s">
+        <v>266</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
     </row>
     <row r="77" spans="1:2">
-      <c r="A77" s="1" t="s">
-        <v>269</v>
+      <c r="A77" s="2" t="s">
+        <v>504</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>175</v>
+        <v>141</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" s="1" t="s">
         <v>394</v>
       </c>
-      <c r="B80" s="1" t="s">
+      <c r="B82" s="1" t="s">
         <v>169</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:B79">
-    <sortCondition ref="A2:A79"/>
+  <sortState ref="A2:B82">
+    <sortCondition ref="A2:A82"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -5298,9 +6275,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A119"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="14.25"/>
   <cols>
@@ -5905,6 +6880,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5912,9 +6888,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B141"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
@@ -7049,6 +8023,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -7056,9 +8031,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -7088,5 +8061,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated config and more documentation
</commit_message>
<xml_diff>
--- a/CRC_Manifest_Processor_Config.xlsx
+++ b/CRC_Manifest_Processor_Config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="19020" windowHeight="11895"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="19020" windowHeight="11895" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="DestinationHubCountry" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1010" uniqueCount="512">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1021" uniqueCount="518">
   <si>
     <t>FINAL_DESTINATION</t>
   </si>
@@ -1554,13 +1554,31 @@
   </si>
   <si>
     <t>CAMP PATRIOT</t>
+  </si>
+  <si>
+    <t>MIKE SPANN</t>
+  </si>
+  <si>
+    <t>MEYMANA</t>
+  </si>
+  <si>
+    <t>MEYMANAH</t>
+  </si>
+  <si>
+    <t>MEHTOR LAM</t>
+  </si>
+  <si>
+    <t>HER AT</t>
+  </si>
+  <si>
+    <t>GADEZ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="23">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1727,6 +1745,12 @@
       <color indexed="8"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="3"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="33">
@@ -2071,7 +2095,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2087,6 +2111,9 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -2445,7 +2472,7 @@
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3381,9 +3408,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C199"/>
+  <dimension ref="A1:C200"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
@@ -5120,9 +5149,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="158" spans="1:3">
-      <c r="A158" s="2" t="s">
-        <v>169</v>
+    <row r="158" spans="1:3" ht="15">
+      <c r="A158" s="8" t="s">
+        <v>512</v>
       </c>
       <c r="B158" s="1" t="s">
         <v>28</v>
@@ -5131,23 +5160,23 @@
         <v>17</v>
       </c>
     </row>
-    <row r="159" spans="1:3">
-      <c r="A159" s="1" t="s">
-        <v>170</v>
+    <row r="159" spans="1:3" ht="15">
+      <c r="A159" s="8" t="s">
+        <v>513</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>171</v>
+        <v>28</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>172</v>
+        <v>17</v>
       </c>
     </row>
     <row r="160" spans="1:3">
       <c r="A160" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="C160" s="1" t="s">
         <v>172</v>
@@ -5155,7 +5184,7 @@
     </row>
     <row r="161" spans="1:3">
       <c r="A161" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B161" s="1" t="s">
         <v>178</v>
@@ -5166,7 +5195,7 @@
     </row>
     <row r="162" spans="1:3">
       <c r="A162" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B162" s="1" t="s">
         <v>178</v>
@@ -5177,7 +5206,7 @@
     </row>
     <row r="163" spans="1:3">
       <c r="A163" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B163" s="1" t="s">
         <v>178</v>
@@ -5188,10 +5217,10 @@
     </row>
     <row r="164" spans="1:3">
       <c r="A164" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C164" s="1" t="s">
         <v>172</v>
@@ -5199,10 +5228,10 @@
     </row>
     <row r="165" spans="1:3">
       <c r="A165" s="1" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C165" s="1" t="s">
         <v>172</v>
@@ -5210,7 +5239,7 @@
     </row>
     <row r="166" spans="1:3">
       <c r="A166" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B166" s="1" t="s">
         <v>178</v>
@@ -5221,7 +5250,7 @@
     </row>
     <row r="167" spans="1:3">
       <c r="A167" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B167" s="1" t="s">
         <v>178</v>
@@ -5232,7 +5261,7 @@
     </row>
     <row r="168" spans="1:3">
       <c r="A168" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B168" s="1" t="s">
         <v>178</v>
@@ -5243,7 +5272,7 @@
     </row>
     <row r="169" spans="1:3">
       <c r="A169" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B169" s="1" t="s">
         <v>178</v>
@@ -5254,10 +5283,10 @@
     </row>
     <row r="170" spans="1:3">
       <c r="A170" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="C170" s="1" t="s">
         <v>172</v>
@@ -5265,10 +5294,10 @@
     </row>
     <row r="171" spans="1:3">
       <c r="A171" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C171" s="1" t="s">
         <v>172</v>
@@ -5276,7 +5305,7 @@
     </row>
     <row r="172" spans="1:3">
       <c r="A172" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B172" s="1" t="s">
         <v>178</v>
@@ -5287,7 +5316,7 @@
     </row>
     <row r="173" spans="1:3">
       <c r="A173" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B173" s="1" t="s">
         <v>178</v>
@@ -5298,7 +5327,7 @@
     </row>
     <row r="174" spans="1:3">
       <c r="A174" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B174" s="1" t="s">
         <v>178</v>
@@ -5309,7 +5338,7 @@
     </row>
     <row r="175" spans="1:3">
       <c r="A175" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B175" s="1" t="s">
         <v>178</v>
@@ -5320,7 +5349,7 @@
     </row>
     <row r="176" spans="1:3">
       <c r="A176" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B176" s="1" t="s">
         <v>178</v>
@@ -5331,10 +5360,10 @@
     </row>
     <row r="177" spans="1:3">
       <c r="A177" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="C177" s="1" t="s">
         <v>172</v>
@@ -5342,10 +5371,10 @@
     </row>
     <row r="178" spans="1:3">
       <c r="A178" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="C178" s="1" t="s">
         <v>172</v>
@@ -5353,10 +5382,10 @@
     </row>
     <row r="179" spans="1:3">
       <c r="A179" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="C179" s="1" t="s">
         <v>172</v>
@@ -5364,10 +5393,10 @@
     </row>
     <row r="180" spans="1:3">
       <c r="A180" s="1" t="s">
-        <v>171</v>
+        <v>193</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="C180" s="1" t="s">
         <v>172</v>
@@ -5375,10 +5404,10 @@
     </row>
     <row r="181" spans="1:3">
       <c r="A181" s="1" t="s">
-        <v>194</v>
+        <v>171</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="C181" s="1" t="s">
         <v>172</v>
@@ -5386,10 +5415,10 @@
     </row>
     <row r="182" spans="1:3">
       <c r="A182" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C182" s="1" t="s">
         <v>172</v>
@@ -5397,7 +5426,7 @@
     </row>
     <row r="183" spans="1:3">
       <c r="A183" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B183" s="1" t="s">
         <v>178</v>
@@ -5408,7 +5437,7 @@
     </row>
     <row r="184" spans="1:3">
       <c r="A184" s="1" t="s">
-        <v>13</v>
+        <v>196</v>
       </c>
       <c r="B184" s="1" t="s">
         <v>178</v>
@@ -5419,7 +5448,7 @@
     </row>
     <row r="185" spans="1:3">
       <c r="A185" s="1" t="s">
-        <v>197</v>
+        <v>13</v>
       </c>
       <c r="B185" s="1" t="s">
         <v>178</v>
@@ -5430,7 +5459,7 @@
     </row>
     <row r="186" spans="1:3">
       <c r="A186" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B186" s="1" t="s">
         <v>178</v>
@@ -5441,18 +5470,18 @@
     </row>
     <row r="187" spans="1:3">
       <c r="A187" s="1" t="s">
-        <v>3</v>
+        <v>198</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>3</v>
+        <v>178</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>4</v>
+        <v>172</v>
       </c>
     </row>
     <row r="188" spans="1:3">
       <c r="A188" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B188" s="1" t="s">
         <v>3</v>
@@ -5463,7 +5492,7 @@
     </row>
     <row r="189" spans="1:3">
       <c r="A189" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B189" s="1" t="s">
         <v>3</v>
@@ -5474,7 +5503,7 @@
     </row>
     <row r="190" spans="1:3">
       <c r="A190" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B190" s="1" t="s">
         <v>3</v>
@@ -5485,7 +5514,7 @@
     </row>
     <row r="191" spans="1:3">
       <c r="A191" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B191" s="1" t="s">
         <v>3</v>
@@ -5496,7 +5525,7 @@
     </row>
     <row r="192" spans="1:3">
       <c r="A192" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B192" s="1" t="s">
         <v>3</v>
@@ -5507,7 +5536,7 @@
     </row>
     <row r="193" spans="1:3">
       <c r="A193" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B193" s="1" t="s">
         <v>3</v>
@@ -5518,7 +5547,7 @@
     </row>
     <row r="194" spans="1:3">
       <c r="A194" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B194" s="1" t="s">
         <v>3</v>
@@ -5529,7 +5558,7 @@
     </row>
     <row r="195" spans="1:3">
       <c r="A195" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B195" s="1" t="s">
         <v>3</v>
@@ -5540,7 +5569,7 @@
     </row>
     <row r="196" spans="1:3">
       <c r="A196" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B196" s="1" t="s">
         <v>3</v>
@@ -5551,7 +5580,7 @@
     </row>
     <row r="197" spans="1:3">
       <c r="A197" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B197" s="1" t="s">
         <v>3</v>
@@ -5562,23 +5591,34 @@
     </row>
     <row r="198" spans="1:3">
       <c r="A198" s="1" t="s">
-        <v>199</v>
+        <v>14</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>199</v>
+        <v>3</v>
       </c>
       <c r="C198" s="1" t="s">
-        <v>200</v>
+        <v>4</v>
       </c>
     </row>
     <row r="199" spans="1:3">
       <c r="A199" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B199" s="1" t="s">
         <v>199</v>
       </c>
       <c r="C199" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3">
+      <c r="A200" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B200" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C200" s="1" t="s">
         <v>200</v>
       </c>
     </row>
@@ -5594,9 +5634,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B82"/>
+  <dimension ref="A1:B86"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
@@ -5813,17 +5855,17 @@
         <v>65</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="1" t="s">
-        <v>223</v>
+    <row r="27" spans="1:2" ht="15">
+      <c r="A27" s="8" t="s">
+        <v>517</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>72</v>
@@ -5831,87 +5873,87 @@
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
-      <c r="A30" s="1" t="s">
-        <v>226</v>
+    <row r="30" spans="1:2" ht="15">
+      <c r="A30" s="8" t="s">
+        <v>516</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>74</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32" s="4" t="s">
-        <v>391</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
     </row>
     <row r="34" spans="1:2">
-      <c r="A34" s="1" t="s">
-        <v>229</v>
+      <c r="A34" s="4" t="s">
+        <v>391</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>151</v>
+        <v>64</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>151</v>
+        <v>64</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>88</v>
+        <v>151</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>88</v>
+        <v>151</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>88</v>
@@ -5919,7 +5961,7 @@
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>88</v>
@@ -5927,31 +5969,31 @@
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="1" t="s">
-        <v>510</v>
+        <v>234</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>10</v>
+        <v>88</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="1" t="s">
-        <v>91</v>
+        <v>510</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>91</v>
+        <v>10</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>91</v>
@@ -5959,7 +6001,7 @@
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="1" t="s">
-        <v>238</v>
+        <v>91</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>91</v>
@@ -5967,63 +6009,63 @@
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>103</v>
@@ -6031,23 +6073,23 @@
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>104</v>
@@ -6055,7 +6097,7 @@
     </row>
     <row r="57" spans="1:2">
       <c r="A57" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>104</v>
@@ -6063,111 +6105,111 @@
     </row>
     <row r="58" spans="1:2">
       <c r="A58" s="1" t="s">
-        <v>108</v>
+        <v>249</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>251</v>
+        <v>104</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2">
-      <c r="A60" s="1" t="s">
-        <v>253</v>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="15">
+      <c r="A60" s="8" t="s">
+        <v>515</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" s="1" t="s">
-        <v>254</v>
+        <v>108</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>110</v>
+        <v>251</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" s="1" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>118</v>
+        <v>251</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" s="1" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>91</v>
+        <v>110</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" s="1" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>91</v>
+        <v>110</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" s="1" t="s">
-        <v>127</v>
+        <v>255</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>251</v>
+        <v>118</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>138</v>
+        <v>91</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>138</v>
+        <v>91</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" s="1" t="s">
-        <v>260</v>
+        <v>127</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>137</v>
+        <v>251</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" s="1" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" s="1" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" s="1" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>137</v>
@@ -6175,90 +6217,122 @@
     </row>
     <row r="72" spans="1:2">
       <c r="A72" s="1" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" s="1" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" s="1" t="s">
-        <v>395</v>
+        <v>263</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="77" spans="1:2">
-      <c r="A77" s="2" t="s">
-        <v>504</v>
+      <c r="A77" s="1" t="s">
+        <v>395</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>175</v>
+        <v>144</v>
       </c>
     </row>
     <row r="80" spans="1:2">
-      <c r="A80" s="1" t="s">
-        <v>270</v>
+      <c r="A80" s="2" t="s">
+        <v>504</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>167</v>
+        <v>151</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" s="1" t="s">
         <v>394</v>
       </c>
-      <c r="B82" s="1" t="s">
+      <c r="B85" s="1" t="s">
         <v>169</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="15">
+      <c r="A86" s="8" t="s">
+        <v>514</v>
+      </c>
+      <c r="B86" s="8" t="s">
+        <v>513</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Allow 0 ULN seats, do not require Instructions
</commit_message>
<xml_diff>
--- a/CRC_Manifest_Processor_Config.xlsx
+++ b/CRC_Manifest_Processor_Config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="19020" windowHeight="11895" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="19020" windowHeight="11895"/>
   </bookViews>
   <sheets>
     <sheet name="DestinationHubCountry" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1021" uniqueCount="518">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1072" uniqueCount="539">
   <si>
     <t>FINAL_DESTINATION</t>
   </si>
@@ -1556,29 +1556,92 @@
     <t>CAMP PATRIOT</t>
   </si>
   <si>
+    <t>SAKARI KAREZ</t>
+  </si>
+  <si>
+    <t>SARKARI KAREZ</t>
+  </si>
+  <si>
+    <t>SAHKARI KAREZ</t>
+  </si>
+  <si>
+    <t>ENDIST NORTH</t>
+  </si>
+  <si>
+    <t>SHINDAD</t>
+  </si>
+  <si>
+    <t>JALLALABAD</t>
+  </si>
+  <si>
+    <t>BAGHRAM</t>
+  </si>
+  <si>
     <t>MIKE SPANN</t>
   </si>
   <si>
-    <t>MEYMANA</t>
-  </si>
-  <si>
-    <t>MEYMANAH</t>
-  </si>
-  <si>
-    <t>MEHTOR LAM</t>
-  </si>
-  <si>
-    <t>HER AT</t>
-  </si>
-  <si>
-    <t>GADEZ</t>
+    <t>NIKE SPANN</t>
+  </si>
+  <si>
+    <t>ASADABAD</t>
+  </si>
+  <si>
+    <t>KADUNZ</t>
+  </si>
+  <si>
+    <t>LAWTOW</t>
+  </si>
+  <si>
+    <t>ABAD</t>
+  </si>
+  <si>
+    <t>SOLERNO</t>
+  </si>
+  <si>
+    <t>LEATHER NECK</t>
+  </si>
+  <si>
+    <t>LAGMAN QALAT</t>
+  </si>
+  <si>
+    <t>KAF</t>
+  </si>
+  <si>
+    <t>BAF</t>
+  </si>
+  <si>
+    <t>NEW KABUL COMPOUND</t>
+  </si>
+  <si>
+    <t>PROSPERTY</t>
+  </si>
+  <si>
+    <t>SABALU-HARRISON</t>
+  </si>
+  <si>
+    <t>FAZAH</t>
+  </si>
+  <si>
+    <t>SHARNA</t>
+  </si>
+  <si>
+    <t>TURKHAM</t>
+  </si>
+  <si>
+    <t>EDGERTON</t>
+  </si>
+  <si>
+    <t>EGGLSTON</t>
+  </si>
+  <si>
+    <t>DOHA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="24">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1745,12 +1808,6 @@
       <color indexed="8"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="3"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="33">
@@ -2095,7 +2152,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2111,9 +2168,6 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -2172,13 +2226,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>54</xdr:row>
+      <xdr:row>56</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2572,7 +2626,7 @@
               <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
               <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
             </a:rPr>
-            <a:t>:  Many of the names of final destinations in theater come from other languages (Arabic, Farsi, Pashtu, Urdu, etc.).  Since these languages have non-English alphabets, we use the way the name sounds to create an English spelling for the name.  In many cases there are multiple correct spellings for a location.  For example, see the "other names" from this Wikipedia article:  http://en.wikipedia.org/wiki/Khanashin</a:t>
+            <a:t>:  Many of the names of final destinations in theater come from other languages (Arabic, Farsi, Pashtu, Urdu, etc.).  Since these languages have non-Roman alphabets, we use the way the name sounds to create an English spelling for the name.  In many cases there are multiple correct spellings for a location.  For example, see the "other names" from this Wikipedia article:  http://en.wikipedia.org/wiki/Khanashin</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1200">
             <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
@@ -2937,7 +2991,25 @@
               <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
               <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
             </a:rPr>
-            <a:t> sheet has a list of all of the rank abbrevations for each branch of the US Armed Forces and also DoD Civilian pay grades.</a:t>
+            <a:t> sheet has a list of all of the rank </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t>abbreviations</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" u="none" baseline="0">
+              <a:latin typeface="Consolas" pitchFamily="49" charset="0"/>
+              <a:cs typeface="Consolas" pitchFamily="49" charset="0"/>
+            </a:rPr>
+            <a:t> for each branch of the US Armed Forces and also DoD Civilian pay grades.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -3408,11 +3480,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C200"/>
+  <dimension ref="A1:C207"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
@@ -3435,7 +3505,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>15</v>
+        <v>524</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>16</v>
@@ -3446,7 +3516,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>16</v>
@@ -3457,7 +3527,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>16</v>
@@ -3468,7 +3538,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>16</v>
@@ -3479,7 +3549,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>16</v>
@@ -3490,10 +3560,10 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>17</v>
@@ -3501,7 +3571,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>23</v>
@@ -3512,7 +3582,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>23</v>
@@ -3523,7 +3593,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>23</v>
@@ -3534,10 +3604,10 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
-        <v>27</v>
+        <v>521</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>17</v>
@@ -3545,10 +3615,10 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>17</v>
@@ -3556,10 +3626,10 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>17</v>
@@ -3567,10 +3637,10 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>17</v>
@@ -3578,10 +3648,10 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>17</v>
@@ -3589,10 +3659,10 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>17</v>
@@ -3600,10 +3670,10 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>17</v>
@@ -3611,10 +3681,10 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>17</v>
@@ -3622,10 +3692,10 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>17</v>
@@ -3633,10 +3703,10 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>17</v>
@@ -3644,10 +3714,10 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>17</v>
@@ -3655,10 +3725,10 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>17</v>
@@ -3666,10 +3736,10 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>17</v>
@@ -3677,10 +3747,10 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>17</v>
@@ -3688,10 +3758,10 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>17</v>
@@ -3699,10 +3769,10 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>17</v>
@@ -3710,7 +3780,7 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>16</v>
@@ -3721,7 +3791,7 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>16</v>
@@ -3732,7 +3802,7 @@
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>16</v>
@@ -3743,10 +3813,10 @@
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>17</v>
@@ -3754,10 +3824,10 @@
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>17</v>
@@ -3765,10 +3835,10 @@
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>17</v>
@@ -3776,7 +3846,7 @@
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>23</v>
@@ -3787,10 +3857,10 @@
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>17</v>
@@ -3798,7 +3868,7 @@
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>23</v>
@@ -3809,10 +3879,10 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>17</v>
@@ -3820,10 +3890,10 @@
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>17</v>
@@ -3831,7 +3901,7 @@
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="1" t="s">
-        <v>54</v>
+        <v>536</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>23</v>
@@ -3841,11 +3911,11 @@
       </c>
     </row>
     <row r="39" spans="1:3">
-      <c r="A39" s="2" t="s">
-        <v>392</v>
+      <c r="A39" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>17</v>
@@ -3853,10 +3923,10 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>17</v>
@@ -3864,10 +3934,10 @@
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="1" t="s">
-        <v>56</v>
+        <v>515</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>17</v>
@@ -3875,21 +3945,21 @@
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="43" spans="1:3">
-      <c r="A43" s="1" t="s">
-        <v>58</v>
+      <c r="A43" s="2" t="s">
+        <v>392</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>17</v>
@@ -3897,10 +3967,10 @@
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>17</v>
@@ -3908,7 +3978,7 @@
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>28</v>
@@ -3919,10 +3989,10 @@
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>17</v>
@@ -3930,10 +4000,10 @@
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>17</v>
@@ -3941,7 +4011,7 @@
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>28</v>
@@ -3952,10 +4022,10 @@
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>17</v>
@@ -3963,10 +4033,10 @@
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>17</v>
@@ -3974,10 +4044,10 @@
     </row>
     <row r="51" spans="1:3">
       <c r="A51" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>17</v>
@@ -3985,7 +4055,7 @@
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>28</v>
@@ -3996,7 +4066,7 @@
     </row>
     <row r="53" spans="1:3">
       <c r="A53" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>23</v>
@@ -4007,10 +4077,10 @@
     </row>
     <row r="54" spans="1:3">
       <c r="A54" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>17</v>
@@ -4018,10 +4088,10 @@
     </row>
     <row r="55" spans="1:3">
       <c r="A55" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>17</v>
@@ -4029,10 +4099,10 @@
     </row>
     <row r="56" spans="1:3">
       <c r="A56" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>17</v>
@@ -4040,10 +4110,10 @@
     </row>
     <row r="57" spans="1:3">
       <c r="A57" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>17</v>
@@ -4051,10 +4121,10 @@
     </row>
     <row r="58" spans="1:3">
       <c r="A58" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>17</v>
@@ -4062,7 +4132,7 @@
     </row>
     <row r="59" spans="1:3">
       <c r="A59" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>23</v>
@@ -4073,10 +4143,10 @@
     </row>
     <row r="60" spans="1:3">
       <c r="A60" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>17</v>
@@ -4084,10 +4154,10 @@
     </row>
     <row r="61" spans="1:3">
       <c r="A61" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>17</v>
@@ -4095,10 +4165,10 @@
     </row>
     <row r="62" spans="1:3">
       <c r="A62" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>17</v>
@@ -4106,7 +4176,7 @@
     </row>
     <row r="63" spans="1:3">
       <c r="A63" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>23</v>
@@ -4117,10 +4187,10 @@
     </row>
     <row r="64" spans="1:3">
       <c r="A64" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>17</v>
@@ -4128,7 +4198,7 @@
     </row>
     <row r="65" spans="1:3">
       <c r="A65" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>23</v>
@@ -4139,10 +4209,10 @@
     </row>
     <row r="66" spans="1:3">
       <c r="A66" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>17</v>
@@ -4150,7 +4220,7 @@
     </row>
     <row r="67" spans="1:3">
       <c r="A67" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>23</v>
@@ -4161,10 +4231,10 @@
     </row>
     <row r="68" spans="1:3">
       <c r="A68" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>17</v>
@@ -4172,10 +4242,10 @@
     </row>
     <row r="69" spans="1:3">
       <c r="A69" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>17</v>
@@ -4183,10 +4253,10 @@
     </row>
     <row r="70" spans="1:3">
       <c r="A70" s="1" t="s">
-        <v>16</v>
+        <v>81</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>17</v>
@@ -4194,7 +4264,7 @@
     </row>
     <row r="71" spans="1:3">
       <c r="A71" s="1" t="s">
-        <v>23</v>
+        <v>82</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>23</v>
@@ -4205,10 +4275,10 @@
     </row>
     <row r="72" spans="1:3">
       <c r="A72" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>17</v>
@@ -4216,10 +4286,10 @@
     </row>
     <row r="73" spans="1:3">
       <c r="A73" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>17</v>
@@ -4227,10 +4297,10 @@
     </row>
     <row r="74" spans="1:3">
       <c r="A74" s="1" t="s">
-        <v>88</v>
+        <v>16</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>17</v>
@@ -4238,10 +4308,10 @@
     </row>
     <row r="75" spans="1:3">
       <c r="A75" s="1" t="s">
-        <v>89</v>
+        <v>23</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>17</v>
@@ -4249,10 +4319,10 @@
     </row>
     <row r="76" spans="1:3">
       <c r="A76" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>17</v>
@@ -4260,7 +4330,7 @@
     </row>
     <row r="77" spans="1:3">
       <c r="A77" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>28</v>
@@ -4271,7 +4341,7 @@
     </row>
     <row r="78" spans="1:3">
       <c r="A78" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>23</v>
@@ -4282,10 +4352,10 @@
     </row>
     <row r="79" spans="1:3">
       <c r="A79" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>17</v>
@@ -4293,10 +4363,10 @@
     </row>
     <row r="80" spans="1:3">
       <c r="A80" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>17</v>
@@ -4304,10 +4374,10 @@
     </row>
     <row r="81" spans="1:3">
       <c r="A81" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>17</v>
@@ -4315,10 +4385,10 @@
     </row>
     <row r="82" spans="1:3">
       <c r="A82" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>17</v>
@@ -4326,7 +4396,7 @@
     </row>
     <row r="83" spans="1:3">
       <c r="A83" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>16</v>
@@ -4337,7 +4407,7 @@
     </row>
     <row r="84" spans="1:3">
       <c r="A84" s="1" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>23</v>
@@ -4348,7 +4418,7 @@
     </row>
     <row r="85" spans="1:3">
       <c r="A85" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>23</v>
@@ -4359,10 +4429,10 @@
     </row>
     <row r="86" spans="1:3">
       <c r="A86" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>17</v>
@@ -4370,10 +4440,10 @@
     </row>
     <row r="87" spans="1:3">
       <c r="A87" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>17</v>
@@ -4381,7 +4451,7 @@
     </row>
     <row r="88" spans="1:3">
       <c r="A88" s="1" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>23</v>
@@ -4392,10 +4462,10 @@
     </row>
     <row r="89" spans="1:3">
       <c r="A89" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>17</v>
@@ -4403,10 +4473,10 @@
     </row>
     <row r="90" spans="1:3">
       <c r="A90" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>17</v>
@@ -4414,10 +4484,10 @@
     </row>
     <row r="91" spans="1:3">
       <c r="A91" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>17</v>
@@ -4425,7 +4495,7 @@
     </row>
     <row r="92" spans="1:3">
       <c r="A92" s="1" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>23</v>
@@ -4436,10 +4506,10 @@
     </row>
     <row r="93" spans="1:3">
       <c r="A93" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>17</v>
@@ -4447,7 +4517,7 @@
     </row>
     <row r="94" spans="1:3">
       <c r="A94" s="1" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>28</v>
@@ -4458,10 +4528,10 @@
     </row>
     <row r="95" spans="1:3">
       <c r="A95" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>17</v>
@@ -4469,7 +4539,7 @@
     </row>
     <row r="96" spans="1:3">
       <c r="A96" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>23</v>
@@ -4480,10 +4550,10 @@
     </row>
     <row r="97" spans="1:3">
       <c r="A97" s="1" t="s">
-        <v>110</v>
+        <v>519</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>17</v>
@@ -4491,10 +4561,10 @@
     </row>
     <row r="98" spans="1:3">
       <c r="A98" s="1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>17</v>
@@ -4502,10 +4572,10 @@
     </row>
     <row r="99" spans="1:3">
       <c r="A99" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>17</v>
@@ -4513,7 +4583,7 @@
     </row>
     <row r="100" spans="1:3">
       <c r="A100" s="1" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>23</v>
@@ -4524,10 +4594,10 @@
     </row>
     <row r="101" spans="1:3">
       <c r="A101" s="1" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>17</v>
@@ -4535,10 +4605,10 @@
     </row>
     <row r="102" spans="1:3">
       <c r="A102" s="1" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C102" s="1" t="s">
         <v>17</v>
@@ -4546,10 +4616,10 @@
     </row>
     <row r="103" spans="1:3">
       <c r="A103" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>17</v>
@@ -4557,10 +4627,10 @@
     </row>
     <row r="104" spans="1:3">
       <c r="A104" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>17</v>
@@ -4568,10 +4638,10 @@
     </row>
     <row r="105" spans="1:3">
       <c r="A105" s="1" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>17</v>
@@ -4579,21 +4649,21 @@
     </row>
     <row r="106" spans="1:3">
       <c r="A106" s="1" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="107" spans="1:3">
-      <c r="A107" s="2" t="s">
-        <v>393</v>
+      <c r="A107" s="1" t="s">
+        <v>115</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C107" s="1" t="s">
         <v>17</v>
@@ -4601,10 +4671,10 @@
     </row>
     <row r="108" spans="1:3">
       <c r="A108" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C108" s="1" t="s">
         <v>17</v>
@@ -4612,10 +4682,10 @@
     </row>
     <row r="109" spans="1:3">
       <c r="A109" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C109" s="1" t="s">
         <v>17</v>
@@ -4623,7 +4693,7 @@
     </row>
     <row r="110" spans="1:3">
       <c r="A110" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>28</v>
@@ -4634,7 +4704,7 @@
     </row>
     <row r="111" spans="1:3">
       <c r="A111" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>28</v>
@@ -4644,11 +4714,11 @@
       </c>
     </row>
     <row r="112" spans="1:3">
-      <c r="A112" s="1" t="s">
-        <v>124</v>
+      <c r="A112" s="2" t="s">
+        <v>393</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>17</v>
@@ -4656,10 +4726,10 @@
     </row>
     <row r="113" spans="1:3">
       <c r="A113" s="1" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>17</v>
@@ -4667,10 +4737,10 @@
     </row>
     <row r="114" spans="1:3">
       <c r="A114" s="1" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>17</v>
@@ -4678,10 +4748,10 @@
     </row>
     <row r="115" spans="1:3">
       <c r="A115" s="1" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C115" s="1" t="s">
         <v>17</v>
@@ -4689,10 +4759,10 @@
     </row>
     <row r="116" spans="1:3">
       <c r="A116" s="1" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C116" s="1" t="s">
         <v>17</v>
@@ -4700,7 +4770,7 @@
     </row>
     <row r="117" spans="1:3">
       <c r="A117" s="1" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>23</v>
@@ -4711,10 +4781,10 @@
     </row>
     <row r="118" spans="1:3">
       <c r="A118" s="1" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C118" s="1" t="s">
         <v>17</v>
@@ -4722,10 +4792,10 @@
     </row>
     <row r="119" spans="1:3">
       <c r="A119" s="1" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C119" s="1" t="s">
         <v>17</v>
@@ -4733,10 +4803,10 @@
     </row>
     <row r="120" spans="1:3">
       <c r="A120" s="1" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C120" s="1" t="s">
         <v>17</v>
@@ -4744,10 +4814,10 @@
     </row>
     <row r="121" spans="1:3">
       <c r="A121" s="1" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C121" s="1" t="s">
         <v>17</v>
@@ -4755,10 +4825,10 @@
     </row>
     <row r="122" spans="1:3">
       <c r="A122" s="1" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C122" s="1" t="s">
         <v>17</v>
@@ -4766,7 +4836,7 @@
     </row>
     <row r="123" spans="1:3">
       <c r="A123" s="1" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>23</v>
@@ -4777,18 +4847,18 @@
     </row>
     <row r="124" spans="1:3">
       <c r="A124" s="1" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C124" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="125" spans="1:3">
-      <c r="A125" s="1" t="s">
-        <v>137</v>
+      <c r="A125" s="2" t="s">
+        <v>532</v>
       </c>
       <c r="B125" s="1" t="s">
         <v>16</v>
@@ -4799,7 +4869,7 @@
     </row>
     <row r="126" spans="1:3">
       <c r="A126" s="1" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B126" s="1" t="s">
         <v>16</v>
@@ -4810,10 +4880,10 @@
     </row>
     <row r="127" spans="1:3">
       <c r="A127" s="1" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="C127" s="1" t="s">
         <v>17</v>
@@ -4821,7 +4891,7 @@
     </row>
     <row r="128" spans="1:3">
       <c r="A128" s="1" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B128" s="1" t="s">
         <v>28</v>
@@ -4832,10 +4902,10 @@
     </row>
     <row r="129" spans="1:3">
       <c r="A129" s="1" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C129" s="1" t="s">
         <v>17</v>
@@ -4843,7 +4913,7 @@
     </row>
     <row r="130" spans="1:3">
       <c r="A130" s="1" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="B130" s="1" t="s">
         <v>23</v>
@@ -4854,7 +4924,7 @@
     </row>
     <row r="131" spans="1:3">
       <c r="A131" s="1" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B131" s="1" t="s">
         <v>16</v>
@@ -4865,7 +4935,7 @@
     </row>
     <row r="132" spans="1:3">
       <c r="A132" s="1" t="s">
-        <v>144</v>
+        <v>513</v>
       </c>
       <c r="B132" s="1" t="s">
         <v>23</v>
@@ -4876,10 +4946,10 @@
     </row>
     <row r="133" spans="1:3">
       <c r="A133" s="1" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="C133" s="1" t="s">
         <v>17</v>
@@ -4887,10 +4957,10 @@
     </row>
     <row r="134" spans="1:3">
       <c r="A134" s="1" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C134" s="1" t="s">
         <v>17</v>
@@ -4898,7 +4968,7 @@
     </row>
     <row r="135" spans="1:3">
       <c r="A135" s="1" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="B135" s="1" t="s">
         <v>28</v>
@@ -4909,10 +4979,10 @@
     </row>
     <row r="136" spans="1:3">
       <c r="A136" s="1" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C136" s="1" t="s">
         <v>17</v>
@@ -4920,7 +4990,7 @@
     </row>
     <row r="137" spans="1:3">
       <c r="A137" s="1" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="B137" s="1" t="s">
         <v>23</v>
@@ -4931,10 +5001,10 @@
     </row>
     <row r="138" spans="1:3">
       <c r="A138" s="1" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C138" s="1" t="s">
         <v>17</v>
@@ -4942,10 +5012,10 @@
     </row>
     <row r="139" spans="1:3">
       <c r="A139" s="1" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C139" s="1" t="s">
         <v>17</v>
@@ -4953,10 +5023,10 @@
     </row>
     <row r="140" spans="1:3">
       <c r="A140" s="1" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="C140" s="1" t="s">
         <v>17</v>
@@ -4964,10 +5034,10 @@
     </row>
     <row r="141" spans="1:3">
       <c r="A141" s="1" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="C141" s="1" t="s">
         <v>17</v>
@@ -4975,10 +5045,10 @@
     </row>
     <row r="142" spans="1:3">
       <c r="A142" s="1" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="C142" s="1" t="s">
         <v>17</v>
@@ -4986,7 +5056,7 @@
     </row>
     <row r="143" spans="1:3">
       <c r="A143" s="1" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="B143" s="1" t="s">
         <v>23</v>
@@ -4997,10 +5067,10 @@
     </row>
     <row r="144" spans="1:3">
       <c r="A144" s="1" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C144" s="1" t="s">
         <v>17</v>
@@ -5008,10 +5078,10 @@
     </row>
     <row r="145" spans="1:3">
       <c r="A145" s="1" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C145" s="1" t="s">
         <v>17</v>
@@ -5019,10 +5089,10 @@
     </row>
     <row r="146" spans="1:3">
       <c r="A146" s="1" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C146" s="1" t="s">
         <v>17</v>
@@ -5030,7 +5100,7 @@
     </row>
     <row r="147" spans="1:3">
       <c r="A147" s="1" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="B147" s="1" t="s">
         <v>23</v>
@@ -5041,10 +5111,10 @@
     </row>
     <row r="148" spans="1:3">
       <c r="A148" s="1" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C148" s="1" t="s">
         <v>17</v>
@@ -5052,7 +5122,7 @@
     </row>
     <row r="149" spans="1:3">
       <c r="A149" s="1" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="B149" s="1" t="s">
         <v>16</v>
@@ -5063,7 +5133,7 @@
     </row>
     <row r="150" spans="1:3">
       <c r="A150" s="1" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="B150" s="1" t="s">
         <v>23</v>
@@ -5074,7 +5144,7 @@
     </row>
     <row r="151" spans="1:3">
       <c r="A151" s="1" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="B151" s="1" t="s">
         <v>28</v>
@@ -5085,7 +5155,7 @@
     </row>
     <row r="152" spans="1:3">
       <c r="A152" s="1" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="B152" s="1" t="s">
         <v>28</v>
@@ -5096,10 +5166,10 @@
     </row>
     <row r="153" spans="1:3">
       <c r="A153" s="1" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C153" s="1" t="s">
         <v>17</v>
@@ -5107,7 +5177,7 @@
     </row>
     <row r="154" spans="1:3">
       <c r="A154" s="1" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="B154" s="1" t="s">
         <v>23</v>
@@ -5118,10 +5188,10 @@
     </row>
     <row r="155" spans="1:3">
       <c r="A155" s="1" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C155" s="1" t="s">
         <v>17</v>
@@ -5129,7 +5199,7 @@
     </row>
     <row r="156" spans="1:3">
       <c r="A156" s="1" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="B156" s="1" t="s">
         <v>16</v>
@@ -5140,18 +5210,18 @@
     </row>
     <row r="157" spans="1:3">
       <c r="A157" s="1" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C157" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="158" spans="1:3" ht="15">
-      <c r="A158" s="8" t="s">
-        <v>512</v>
+    <row r="158" spans="1:3">
+      <c r="A158" s="1" t="s">
+        <v>163</v>
       </c>
       <c r="B158" s="1" t="s">
         <v>28</v>
@@ -5160,9 +5230,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="159" spans="1:3" ht="15">
-      <c r="A159" s="8" t="s">
-        <v>513</v>
+    <row r="159" spans="1:3">
+      <c r="A159" s="1" t="s">
+        <v>164</v>
       </c>
       <c r="B159" s="1" t="s">
         <v>28</v>
@@ -5173,76 +5243,76 @@
     </row>
     <row r="160" spans="1:3">
       <c r="A160" s="1" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>171</v>
+        <v>28</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>172</v>
+        <v>17</v>
       </c>
     </row>
     <row r="161" spans="1:3">
       <c r="A161" s="1" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>178</v>
+        <v>23</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>172</v>
+        <v>17</v>
       </c>
     </row>
     <row r="162" spans="1:3">
       <c r="A162" s="1" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>178</v>
+        <v>34</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>172</v>
+        <v>17</v>
       </c>
     </row>
     <row r="163" spans="1:3">
       <c r="A163" s="1" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>178</v>
+        <v>16</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>172</v>
+        <v>17</v>
       </c>
     </row>
     <row r="164" spans="1:3">
       <c r="A164" s="1" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>178</v>
+        <v>16</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>172</v>
+        <v>17</v>
       </c>
     </row>
     <row r="165" spans="1:3">
-      <c r="A165" s="1" t="s">
-        <v>179</v>
+      <c r="A165" s="2" t="s">
+        <v>169</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>179</v>
+        <v>28</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>172</v>
+        <v>17</v>
       </c>
     </row>
     <row r="166" spans="1:3">
       <c r="A166" s="1" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="C166" s="1" t="s">
         <v>172</v>
@@ -5250,7 +5320,7 @@
     </row>
     <row r="167" spans="1:3">
       <c r="A167" s="1" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="B167" s="1" t="s">
         <v>178</v>
@@ -5261,7 +5331,7 @@
     </row>
     <row r="168" spans="1:3">
       <c r="A168" s="1" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="B168" s="1" t="s">
         <v>178</v>
@@ -5272,7 +5342,7 @@
     </row>
     <row r="169" spans="1:3">
       <c r="A169" s="1" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="B169" s="1" t="s">
         <v>178</v>
@@ -5283,7 +5353,7 @@
     </row>
     <row r="170" spans="1:3">
       <c r="A170" s="1" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="B170" s="1" t="s">
         <v>178</v>
@@ -5294,10 +5364,10 @@
     </row>
     <row r="171" spans="1:3">
       <c r="A171" s="1" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="C171" s="1" t="s">
         <v>172</v>
@@ -5305,7 +5375,7 @@
     </row>
     <row r="172" spans="1:3">
       <c r="A172" s="1" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="B172" s="1" t="s">
         <v>178</v>
@@ -5316,7 +5386,7 @@
     </row>
     <row r="173" spans="1:3">
       <c r="A173" s="1" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="B173" s="1" t="s">
         <v>178</v>
@@ -5327,7 +5397,7 @@
     </row>
     <row r="174" spans="1:3">
       <c r="A174" s="1" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="B174" s="1" t="s">
         <v>178</v>
@@ -5338,7 +5408,7 @@
     </row>
     <row r="175" spans="1:3">
       <c r="A175" s="1" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="B175" s="1" t="s">
         <v>178</v>
@@ -5349,7 +5419,7 @@
     </row>
     <row r="176" spans="1:3">
       <c r="A176" s="1" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="B176" s="1" t="s">
         <v>178</v>
@@ -5360,10 +5430,10 @@
     </row>
     <row r="177" spans="1:3">
       <c r="A177" s="1" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C177" s="1" t="s">
         <v>172</v>
@@ -5371,10 +5441,10 @@
     </row>
     <row r="178" spans="1:3">
       <c r="A178" s="1" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="C178" s="1" t="s">
         <v>172</v>
@@ -5382,7 +5452,7 @@
     </row>
     <row r="179" spans="1:3">
       <c r="A179" s="1" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="B179" s="1" t="s">
         <v>178</v>
@@ -5393,10 +5463,10 @@
     </row>
     <row r="180" spans="1:3">
       <c r="A180" s="1" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="C180" s="1" t="s">
         <v>172</v>
@@ -5404,10 +5474,10 @@
     </row>
     <row r="181" spans="1:3">
       <c r="A181" s="1" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="C181" s="1" t="s">
         <v>172</v>
@@ -5415,10 +5485,10 @@
     </row>
     <row r="182" spans="1:3">
       <c r="A182" s="1" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C182" s="1" t="s">
         <v>172</v>
@@ -5426,7 +5496,7 @@
     </row>
     <row r="183" spans="1:3">
       <c r="A183" s="1" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="B183" s="1" t="s">
         <v>178</v>
@@ -5437,10 +5507,10 @@
     </row>
     <row r="184" spans="1:3">
       <c r="A184" s="1" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="C184" s="1" t="s">
         <v>172</v>
@@ -5448,7 +5518,7 @@
     </row>
     <row r="185" spans="1:3">
       <c r="A185" s="1" t="s">
-        <v>13</v>
+        <v>192</v>
       </c>
       <c r="B185" s="1" t="s">
         <v>178</v>
@@ -5459,10 +5529,10 @@
     </row>
     <row r="186" spans="1:3">
       <c r="A186" s="1" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C186" s="1" t="s">
         <v>172</v>
@@ -5470,10 +5540,10 @@
     </row>
     <row r="187" spans="1:3">
       <c r="A187" s="1" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="C187" s="1" t="s">
         <v>172</v>
@@ -5481,73 +5551,73 @@
     </row>
     <row r="188" spans="1:3">
       <c r="A188" s="1" t="s">
-        <v>3</v>
+        <v>194</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>3</v>
+        <v>179</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>4</v>
+        <v>172</v>
       </c>
     </row>
     <row r="189" spans="1:3">
       <c r="A189" s="1" t="s">
-        <v>5</v>
+        <v>195</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>3</v>
+        <v>178</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>4</v>
+        <v>172</v>
       </c>
     </row>
     <row r="190" spans="1:3">
       <c r="A190" s="1" t="s">
-        <v>6</v>
+        <v>196</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>3</v>
+        <v>178</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>4</v>
+        <v>172</v>
       </c>
     </row>
     <row r="191" spans="1:3">
       <c r="A191" s="1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>3</v>
+        <v>178</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>4</v>
+        <v>172</v>
       </c>
     </row>
     <row r="192" spans="1:3">
       <c r="A192" s="1" t="s">
-        <v>8</v>
+        <v>197</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>3</v>
+        <v>178</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>4</v>
+        <v>172</v>
       </c>
     </row>
     <row r="193" spans="1:3">
       <c r="A193" s="1" t="s">
-        <v>9</v>
+        <v>198</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>3</v>
+        <v>178</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>4</v>
+        <v>172</v>
       </c>
     </row>
     <row r="194" spans="1:3">
       <c r="A194" s="1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B194" s="1" t="s">
         <v>3</v>
@@ -5558,7 +5628,7 @@
     </row>
     <row r="195" spans="1:3">
       <c r="A195" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B195" s="1" t="s">
         <v>3</v>
@@ -5569,7 +5639,7 @@
     </row>
     <row r="196" spans="1:3">
       <c r="A196" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B196" s="1" t="s">
         <v>3</v>
@@ -5580,7 +5650,7 @@
     </row>
     <row r="197" spans="1:3">
       <c r="A197" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B197" s="1" t="s">
         <v>3</v>
@@ -5591,7 +5661,7 @@
     </row>
     <row r="198" spans="1:3">
       <c r="A198" s="1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B198" s="1" t="s">
         <v>3</v>
@@ -5602,30 +5672,107 @@
     </row>
     <row r="199" spans="1:3">
       <c r="A199" s="1" t="s">
-        <v>199</v>
+        <v>9</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>199</v>
+        <v>3</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>200</v>
+        <v>4</v>
       </c>
     </row>
     <row r="200" spans="1:3">
       <c r="A200" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B200" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C200" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3">
+      <c r="A201" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B201" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C201" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3">
+      <c r="A202" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B202" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C202" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3">
+      <c r="A203" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B203" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C203" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3">
+      <c r="A204" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B204" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C204" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3">
+      <c r="A205" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B205" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C205" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3">
+      <c r="A206" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="B200" s="1" t="s">
+      <c r="B206" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="C200" s="1" t="s">
+      <c r="C206" s="1" t="s">
         <v>200</v>
       </c>
     </row>
+    <row r="207" spans="1:3">
+      <c r="A207" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="B207" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="C207" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A2:C199">
-    <sortCondition ref="C2:C199"/>
-    <sortCondition ref="A2:A199"/>
+  <sortState ref="A2:C207">
+    <sortCondition ref="C2:C207"/>
+    <sortCondition ref="A2:A207"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5634,11 +5781,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B86"/>
+  <dimension ref="A1:B101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
@@ -5673,39 +5818,39 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>509</v>
+        <v>529</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>178</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>174</v>
+        <v>509</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="1" t="s">
-        <v>506</v>
+      <c r="A6" s="2" t="s">
+        <v>518</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>179</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>205</v>
+        <v>174</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>34</v>
+        <v>184</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="2" t="s">
-        <v>505</v>
+      <c r="A8" s="1" t="s">
+        <v>506</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>179</v>
@@ -5713,55 +5858,55 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="1" t="s">
-        <v>511</v>
+      <c r="A10" s="2" t="s">
+        <v>505</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>10</v>
+        <v>179</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>208</v>
+        <v>511</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>45</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>50</v>
@@ -5769,7 +5914,7 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>50</v>
@@ -5777,7 +5922,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>50</v>
@@ -5785,7 +5930,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>50</v>
@@ -5793,7 +5938,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>50</v>
@@ -5801,39 +5946,39 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>50</v>
@@ -5841,55 +5986,55 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="15">
-      <c r="A27" s="8" t="s">
-        <v>517</v>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="2" t="s">
+        <v>537</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>60</v>
+        <v>536</v>
       </c>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" s="1" t="s">
-        <v>223</v>
+      <c r="A28" s="2" t="s">
+        <v>533</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="15">
-      <c r="A30" s="8" t="s">
-        <v>516</v>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="1" t="s">
+        <v>222</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>72</v>
@@ -5897,295 +6042,295 @@
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>74</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" s="4" t="s">
-        <v>391</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
     </row>
     <row r="36" spans="1:2">
-      <c r="A36" s="1" t="s">
-        <v>229</v>
+      <c r="A36" s="4" t="s">
+        <v>391</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
     </row>
     <row r="37" spans="1:2">
-      <c r="A37" s="1" t="s">
-        <v>230</v>
+      <c r="A37" s="2" t="s">
+        <v>517</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>151</v>
+        <v>81</v>
       </c>
     </row>
     <row r="38" spans="1:2">
-      <c r="A38" s="1" t="s">
-        <v>231</v>
+      <c r="A38" s="2" t="s">
+        <v>522</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>151</v>
+        <v>91</v>
       </c>
     </row>
     <row r="39" spans="1:2">
-      <c r="A39" s="1" t="s">
-        <v>232</v>
+      <c r="A39" s="2" t="s">
+        <v>528</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>88</v>
+        <v>23</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="1" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="1" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="1" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>88</v>
+        <v>151</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="1" t="s">
-        <v>510</v>
+        <v>231</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>10</v>
+        <v>151</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="1" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="1" t="s">
-        <v>91</v>
+        <v>233</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="1" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="1" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="1" t="s">
-        <v>239</v>
+        <v>510</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>105</v>
+        <v>10</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="1" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="1" t="s">
-        <v>241</v>
+        <v>91</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="1" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="1" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
     </row>
     <row r="53" spans="1:2">
-      <c r="A53" s="1" t="s">
-        <v>244</v>
+      <c r="A53" s="2" t="s">
+        <v>527</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
     </row>
     <row r="54" spans="1:2">
-      <c r="A54" s="1" t="s">
-        <v>245</v>
+      <c r="A54" s="2" t="s">
+        <v>523</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="55" spans="1:2">
-      <c r="A55" s="1" t="s">
-        <v>246</v>
+      <c r="A55" s="2" t="s">
+        <v>526</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" s="1" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" s="1" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" s="1" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" s="1" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" ht="15">
-      <c r="A60" s="8" t="s">
-        <v>515</v>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="1" t="s">
+        <v>243</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" s="1" t="s">
-        <v>108</v>
+        <v>244</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>251</v>
+        <v>103</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" s="1" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>251</v>
+        <v>103</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" s="1" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" s="1" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" s="1" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" s="1" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" s="1" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" s="1" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>251</v>
@@ -6193,151 +6338,271 @@
     </row>
     <row r="69" spans="1:2">
       <c r="A69" s="1" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>138</v>
+        <v>251</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" s="1" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>138</v>
+        <v>110</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" s="1" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>137</v>
+        <v>110</v>
       </c>
     </row>
     <row r="72" spans="1:2">
-      <c r="A72" s="1" t="s">
-        <v>261</v>
+      <c r="A72" s="2" t="s">
+        <v>530</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>137</v>
+        <v>16</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" s="1" t="s">
-        <v>262</v>
+        <v>520</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>137</v>
+        <v>519</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" s="1" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>137</v>
+        <v>118</v>
       </c>
     </row>
     <row r="75" spans="1:2">
-      <c r="A75" s="1" t="s">
-        <v>264</v>
+      <c r="A75" s="2" t="s">
+        <v>531</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>138</v>
+        <v>190</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" s="1" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>138</v>
+        <v>91</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" s="1" t="s">
-        <v>395</v>
+        <v>257</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>134</v>
+        <v>91</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" s="1" t="s">
-        <v>266</v>
+        <v>127</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>139</v>
+        <v>251</v>
       </c>
     </row>
     <row r="79" spans="1:2">
-      <c r="A79" s="1" t="s">
-        <v>267</v>
+      <c r="A79" s="2" t="s">
+        <v>514</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>144</v>
+        <v>513</v>
       </c>
     </row>
     <row r="80" spans="1:2">
-      <c r="A80" s="2" t="s">
-        <v>504</v>
+      <c r="A80" s="1" t="s">
+        <v>258</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" s="1" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" s="1" t="s">
-        <v>269</v>
+        <v>512</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>175</v>
+        <v>513</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" s="1" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" s="1" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>167</v>
+        <v>137</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" s="2" t="s">
+        <v>534</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" s="2" t="s">
+        <v>516</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" s="2" t="s">
+        <v>525</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99" s="2" t="s">
+        <v>535</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101" s="1" t="s">
         <v>394</v>
       </c>
-      <c r="B85" s="1" t="s">
+      <c r="B101" s="1" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="15">
-      <c r="A86" s="8" t="s">
-        <v>514</v>
-      </c>
-      <c r="B86" s="8" t="s">
-        <v>513</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState ref="A2:B82">
-    <sortCondition ref="A2:A82"/>
+  <sortState ref="A2:B101">
+    <sortCondition ref="A2:A101"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Strip "AFB" from destinations
</commit_message>
<xml_diff>
--- a/CRC_Manifest_Processor_Config.xlsx
+++ b/CRC_Manifest_Processor_Config.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1072" uniqueCount="539">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1080" uniqueCount="543">
   <si>
     <t>FINAL_DESTINATION</t>
   </si>
@@ -1635,6 +1635,18 @@
   </si>
   <si>
     <t>DOHA</t>
+  </si>
+  <si>
+    <t>KHANDAHAR</t>
+  </si>
+  <si>
+    <t>BAGRAIN</t>
+  </si>
+  <si>
+    <t>ISAF HQ</t>
+  </si>
+  <si>
+    <t>ISAF</t>
   </si>
 </sst>
 </file>
@@ -2152,7 +2164,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2168,6 +2180,9 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -5781,7 +5796,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B101"/>
+  <dimension ref="A1:B105"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5841,64 +5856,64 @@
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="1" t="s">
-        <v>174</v>
+      <c r="A7" s="2" t="s">
+        <v>540</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>184</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
-        <v>506</v>
+        <v>174</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="2" t="s">
+    <row r="11" spans="1:2">
+      <c r="A11" s="2" t="s">
         <v>505</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>179</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>511</v>
+        <v>206</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
-        <v>207</v>
+        <v>511</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>45</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>45</v>
@@ -5906,15 +5921,15 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>50</v>
@@ -5922,7 +5937,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>50</v>
@@ -5930,7 +5945,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>50</v>
@@ -5938,7 +5953,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>50</v>
@@ -5946,7 +5961,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>50</v>
@@ -5954,7 +5969,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>50</v>
@@ -5962,15 +5977,15 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>46</v>
@@ -5978,15 +5993,15 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>50</v>
@@ -5994,55 +6009,55 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="2" t="s">
-        <v>537</v>
+      <c r="A27" s="1" t="s">
+        <v>220</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>536</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="2" t="s">
+        <v>537</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="2" t="s">
         <v>533</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B29" s="1" t="s">
         <v>54</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>72</v>
@@ -6050,7 +6065,7 @@
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>72</v>
@@ -6058,111 +6073,111 @@
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="36" spans="1:2">
-      <c r="A36" s="4" t="s">
-        <v>391</v>
+      <c r="A36" s="1" t="s">
+        <v>227</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="2" t="s">
-        <v>517</v>
+        <v>542</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="2" t="s">
+        <v>541</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="2" t="s">
+        <v>517</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="2" t="s">
         <v>522</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B41" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
-      <c r="A39" s="2" t="s">
+    <row r="42" spans="1:2">
+      <c r="A42" s="2" t="s">
         <v>528</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B42" s="1" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2">
-      <c r="A40" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2">
-      <c r="A41" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2">
-      <c r="A42" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>151</v>
+        <v>64</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="1" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>88</v>
+        <v>151</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>88</v>
+        <v>151</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="1" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>88</v>
@@ -6170,103 +6185,103 @@
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="1" t="s">
-        <v>510</v>
+        <v>233</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>10</v>
+        <v>88</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="50" spans="1:2">
-      <c r="A50" s="1" t="s">
-        <v>91</v>
+      <c r="A50" s="8" t="s">
+        <v>539</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>91</v>
+        <v>23</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="1" t="s">
-        <v>238</v>
+        <v>510</v>
       </c>
       <c r="B52" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B53" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
-      <c r="A53" s="2" t="s">
-        <v>527</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
     <row r="54" spans="1:2">
-      <c r="A54" s="2" t="s">
-        <v>523</v>
+      <c r="A54" s="1" t="s">
+        <v>91</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="55" spans="1:2">
-      <c r="A55" s="2" t="s">
-        <v>526</v>
+      <c r="A55" s="1" t="s">
+        <v>237</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
     </row>
     <row r="57" spans="1:2">
-      <c r="A57" s="1" t="s">
-        <v>240</v>
+      <c r="A57" s="2" t="s">
+        <v>527</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="58" spans="1:2">
-      <c r="A58" s="1" t="s">
-        <v>241</v>
+      <c r="A58" s="2" t="s">
+        <v>523</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="59" spans="1:2">
-      <c r="A59" s="1" t="s">
-        <v>242</v>
+      <c r="A59" s="2" t="s">
+        <v>526</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" s="1" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>105</v>
@@ -6274,335 +6289,367 @@
     </row>
     <row r="61" spans="1:2">
       <c r="A61" s="1" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" s="1" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" s="1" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" s="1" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" s="1" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" s="1" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" s="1" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" s="1" t="s">
-        <v>108</v>
+        <v>247</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>251</v>
+        <v>104</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" s="1" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>251</v>
+        <v>104</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" s="1" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="72" spans="1:2">
-      <c r="A72" s="2" t="s">
-        <v>530</v>
+      <c r="A72" s="1" t="s">
+        <v>108</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>16</v>
+        <v>251</v>
       </c>
     </row>
     <row r="73" spans="1:2">
       <c r="A73" s="1" t="s">
-        <v>520</v>
+        <v>252</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>519</v>
+        <v>251</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
     </row>
     <row r="75" spans="1:2">
-      <c r="A75" s="2" t="s">
-        <v>531</v>
+      <c r="A75" s="1" t="s">
+        <v>254</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>190</v>
+        <v>110</v>
       </c>
     </row>
     <row r="76" spans="1:2">
-      <c r="A76" s="1" t="s">
-        <v>256</v>
+      <c r="A76" s="2" t="s">
+        <v>530</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>91</v>
+        <v>16</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" s="1" t="s">
-        <v>257</v>
+        <v>520</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>91</v>
+        <v>519</v>
       </c>
     </row>
     <row r="78" spans="1:2">
       <c r="A78" s="1" t="s">
-        <v>127</v>
+        <v>255</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>251</v>
+        <v>118</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" s="2" t="s">
-        <v>514</v>
+        <v>531</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>513</v>
+        <v>190</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>138</v>
+        <v>91</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>138</v>
+        <v>91</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" s="1" t="s">
-        <v>512</v>
+        <v>127</v>
       </c>
       <c r="B82" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" s="2" t="s">
+        <v>514</v>
+      </c>
+      <c r="B83" s="1" t="s">
         <v>513</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2">
-      <c r="A83" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" s="1" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" s="1" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" s="1" t="s">
-        <v>263</v>
+        <v>512</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>137</v>
+        <v>513</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" s="1" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" s="1" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" s="1" t="s">
-        <v>395</v>
+        <v>262</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" s="1" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="91" spans="1:2">
-      <c r="A91" s="2" t="s">
-        <v>534</v>
+      <c r="A91" s="1" t="s">
+        <v>264</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="92" spans="1:2">
-      <c r="A92" s="2" t="s">
-        <v>516</v>
+      <c r="A92" s="1" t="s">
+        <v>265</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93" s="1" t="s">
-        <v>267</v>
+        <v>395</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
     </row>
     <row r="94" spans="1:2">
-      <c r="A94" s="2" t="s">
-        <v>504</v>
+      <c r="A94" s="1" t="s">
+        <v>266</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" s="2" t="s">
-        <v>525</v>
+        <v>534</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
     </row>
     <row r="96" spans="1:2">
-      <c r="A96" s="1" t="s">
-        <v>268</v>
+      <c r="A96" s="2" t="s">
+        <v>516</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
     </row>
     <row r="97" spans="1:2">
       <c r="A97" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>175</v>
+        <v>144</v>
       </c>
     </row>
     <row r="98" spans="1:2">
-      <c r="A98" s="1" t="s">
-        <v>270</v>
+      <c r="A98" s="2" t="s">
+        <v>504</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
     </row>
     <row r="99" spans="1:2">
       <c r="A99" s="2" t="s">
-        <v>535</v>
+        <v>525</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>156</v>
+        <v>134</v>
       </c>
     </row>
     <row r="100" spans="1:2">
       <c r="A100" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>167</v>
+        <v>151</v>
       </c>
     </row>
     <row r="101" spans="1:2">
       <c r="A101" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
+      <c r="A102" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" s="2" t="s">
+        <v>535</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105" s="1" t="s">
         <v>394</v>
       </c>
-      <c r="B101" s="1" t="s">
+      <c r="B105" s="1" t="s">
         <v>169</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:B101">
-    <sortCondition ref="A2:A101"/>
+  <sortState ref="A2:B105">
+    <sortCondition ref="A2:A105"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>